<commit_message>
MemoryMap : added piston mov full and zero in the memorymap
</commit_message>
<xml_diff>
--- a/Documentation/MemoryMap/MemoryMap.xlsx
+++ b/Documentation/MemoryMap/MemoryMap.xlsx
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="444" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="447" uniqueCount="113">
   <si>
     <t xml:space="preserve">A</t>
   </si>
@@ -130,6 +130,12 @@
     <t xml:space="preserve">USER_OVERRIDE</t>
   </si>
   <si>
+    <t xml:space="preserve">MOV_ZERO</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MOV_FULL</t>
+  </si>
+  <si>
     <t xml:space="preserve">PST_CAL</t>
   </si>
   <si>
@@ -146,6 +152,9 @@
   </si>
   <si>
     <t xml:space="preserve">0x70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SYS_RST</t>
   </si>
   <si>
     <t xml:space="preserve">0x80</t>
@@ -1708,7 +1717,7 @@
   </sheetPr>
   <dimension ref="A1"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="D60" activeCellId="0" sqref="D60"/>
     </sheetView>
   </sheetViews>
@@ -1731,8 +1740,8 @@
   </sheetPr>
   <dimension ref="B7:R28"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K24" activeCellId="0" sqref="K24"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="H16" activeCellId="0" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.54296875" defaultRowHeight="14.25" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -1965,23 +1974,27 @@
       <c r="F15" s="21" t="s">
         <v>33</v>
       </c>
-      <c r="G15" s="23"/>
-      <c r="H15" s="23"/>
+      <c r="G15" s="21" t="s">
+        <v>34</v>
+      </c>
+      <c r="H15" s="21" t="s">
+        <v>35</v>
+      </c>
       <c r="I15" s="23"/>
       <c r="J15" s="21" t="s">
-        <v>34</v>
+        <v>36</v>
       </c>
       <c r="K15" s="24" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="L15" s="20" t="s">
-        <v>36</v>
+        <v>38</v>
       </c>
       <c r="M15" s="24" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="N15" s="24" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="O15" s="25"/>
       <c r="P15" s="25"/>
@@ -1990,7 +2003,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B16" s="4" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="28"/>
@@ -1999,7 +2012,9 @@
       <c r="G16" s="23"/>
       <c r="H16" s="23"/>
       <c r="I16" s="23"/>
-      <c r="J16" s="23"/>
+      <c r="J16" s="21" t="s">
+        <v>42</v>
+      </c>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
       <c r="M16" s="23"/>
@@ -2011,22 +2026,22 @@
     </row>
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B17" s="4" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C17" s="31" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D17" s="31"/>
       <c r="E17" s="31"/>
       <c r="F17" s="31"/>
       <c r="G17" s="32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H17" s="32"/>
       <c r="I17" s="32"/>
       <c r="J17" s="32"/>
       <c r="K17" s="11" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="L17" s="11"/>
       <c r="M17" s="11"/>
@@ -2038,22 +2053,22 @@
     </row>
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B18" s="4" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C18" s="31" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="D18" s="31"/>
       <c r="E18" s="31"/>
       <c r="F18" s="31"/>
       <c r="G18" s="33" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="H18" s="33"/>
       <c r="I18" s="33"/>
       <c r="J18" s="34"/>
       <c r="K18" s="11" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L18" s="11"/>
       <c r="M18" s="11"/>
@@ -2065,7 +2080,7 @@
     </row>
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B19" s="4" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C19" s="27"/>
       <c r="D19" s="28"/>
@@ -2076,7 +2091,7 @@
       <c r="I19" s="23"/>
       <c r="J19" s="23"/>
       <c r="K19" s="11" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="L19" s="11"/>
       <c r="M19" s="11"/>
@@ -2088,7 +2103,7 @@
     </row>
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B20" s="4" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C20" s="35"/>
       <c r="D20" s="23"/>
@@ -2099,7 +2114,7 @@
       <c r="I20" s="23"/>
       <c r="J20" s="23"/>
       <c r="K20" s="17" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L20" s="17"/>
       <c r="M20" s="17"/>
@@ -2111,7 +2126,7 @@
     </row>
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B21" s="4" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C21" s="36"/>
       <c r="D21" s="37"/>
@@ -2122,7 +2137,7 @@
       <c r="I21" s="37"/>
       <c r="J21" s="37"/>
       <c r="K21" s="11" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="L21" s="11"/>
       <c r="M21" s="11"/>
@@ -2134,7 +2149,7 @@
     </row>
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B22" s="4" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C22" s="27"/>
       <c r="D22" s="28"/>
@@ -2145,7 +2160,7 @@
       <c r="I22" s="23"/>
       <c r="J22" s="23"/>
       <c r="K22" s="17" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L22" s="17"/>
       <c r="M22" s="17"/>
@@ -2157,7 +2172,7 @@
     </row>
     <row r="23" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B23" s="4" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C23" s="35"/>
       <c r="D23" s="23"/>
@@ -2168,7 +2183,7 @@
       <c r="I23" s="23"/>
       <c r="J23" s="23"/>
       <c r="K23" s="20" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="L23" s="20"/>
       <c r="M23" s="20"/>
@@ -2180,10 +2195,10 @@
     </row>
     <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="B24" s="4" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C24" s="38" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="D24" s="38"/>
       <c r="E24" s="38"/>
@@ -2193,17 +2208,17 @@
       <c r="I24" s="38"/>
       <c r="J24" s="38"/>
       <c r="K24" s="20" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="L24" s="20"/>
       <c r="M24" s="39" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="N24" s="39" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="O24" s="20" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="P24" s="20"/>
       <c r="Q24" s="20"/>
@@ -2211,7 +2226,7 @@
     </row>
     <row r="26" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C26" s="40" t="s">
-        <v>64</v>
+        <v>67</v>
       </c>
       <c r="D26" s="40"/>
       <c r="E26" s="40"/>
@@ -2221,7 +2236,7 @@
       <c r="I26" s="40"/>
       <c r="J26" s="40"/>
       <c r="K26" s="41" t="s">
-        <v>65</v>
+        <v>68</v>
       </c>
       <c r="L26" s="41"/>
       <c r="M26" s="41"/>
@@ -2233,7 +2248,7 @@
     </row>
     <row r="28" customFormat="false" ht="14.25" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="C28" s="42" t="s">
-        <v>66</v>
+        <v>69</v>
       </c>
     </row>
   </sheetData>
@@ -2289,7 +2304,7 @@
   </sheetPr>
   <dimension ref="A1:Q35"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="J16" activeCellId="0" sqref="J16"/>
     </sheetView>
   </sheetViews>
@@ -2351,7 +2366,7 @@
         <v>6</v>
       </c>
       <c r="B2" s="49" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="C2" s="49"/>
       <c r="D2" s="49"/>
@@ -2366,16 +2381,16 @@
         <v>6</v>
       </c>
       <c r="I2" s="50" t="s">
-        <v>68</v>
+        <v>71</v>
       </c>
       <c r="J2" s="8" t="s">
-        <v>67</v>
+        <v>70</v>
       </c>
       <c r="K2" s="8"/>
       <c r="L2" s="8"/>
       <c r="M2" s="8"/>
       <c r="N2" s="51" t="s">
-        <v>69</v>
+        <v>72</v>
       </c>
       <c r="O2" s="51"/>
       <c r="P2" s="51"/>
@@ -2410,13 +2425,13 @@
         <v>6</v>
       </c>
       <c r="J3" s="11" t="s">
-        <v>70</v>
+        <v>73</v>
       </c>
       <c r="K3" s="11"/>
       <c r="L3" s="11"/>
       <c r="M3" s="11"/>
       <c r="N3" s="53" t="s">
-        <v>71</v>
+        <v>74</v>
       </c>
       <c r="O3" s="53"/>
       <c r="P3" s="53"/>
@@ -2427,7 +2442,7 @@
         <v>14</v>
       </c>
       <c r="B4" s="55" t="s">
-        <v>72</v>
+        <v>75</v>
       </c>
       <c r="C4" s="55"/>
       <c r="D4" s="55"/>
@@ -2445,13 +2460,13 @@
         <v>6</v>
       </c>
       <c r="J4" s="11" t="s">
-        <v>73</v>
+        <v>76</v>
       </c>
       <c r="K4" s="11"/>
       <c r="L4" s="11"/>
       <c r="M4" s="11"/>
       <c r="N4" s="56" t="s">
-        <v>74</v>
+        <v>77</v>
       </c>
       <c r="O4" s="56"/>
       <c r="P4" s="56"/>
@@ -2486,13 +2501,13 @@
         <v>6</v>
       </c>
       <c r="J5" s="17" t="s">
-        <v>75</v>
+        <v>78</v>
       </c>
       <c r="K5" s="17"/>
       <c r="L5" s="17"/>
       <c r="M5" s="17"/>
       <c r="N5" s="57" t="s">
-        <v>76</v>
+        <v>79</v>
       </c>
       <c r="O5" s="57"/>
       <c r="P5" s="57"/>
@@ -2503,25 +2518,25 @@
         <v>20</v>
       </c>
       <c r="B6" s="55" t="s">
-        <v>77</v>
+        <v>80</v>
       </c>
       <c r="C6" s="55"/>
       <c r="D6" s="55"/>
       <c r="E6" s="55"/>
       <c r="F6" s="14" t="s">
-        <v>78</v>
+        <v>81</v>
       </c>
       <c r="G6" s="14"/>
       <c r="H6" s="14"/>
       <c r="I6" s="14"/>
       <c r="J6" s="20" t="s">
-        <v>79</v>
+        <v>82</v>
       </c>
       <c r="K6" s="20"/>
       <c r="L6" s="20"/>
       <c r="M6" s="20"/>
       <c r="N6" s="56" t="s">
-        <v>80</v>
+        <v>83</v>
       </c>
       <c r="O6" s="56"/>
       <c r="P6" s="56"/>
@@ -2532,7 +2547,7 @@
         <v>25</v>
       </c>
       <c r="B7" s="58" t="s">
-        <v>81</v>
+        <v>84</v>
       </c>
       <c r="C7" s="58"/>
       <c r="D7" s="58"/>
@@ -2579,7 +2594,7 @@
         <v>30</v>
       </c>
       <c r="B8" s="60" t="s">
-        <v>82</v>
+        <v>85</v>
       </c>
       <c r="C8" s="33" t="s">
         <v>6</v>
@@ -2629,7 +2644,7 @@
     </row>
     <row r="9" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B9" s="6" t="s">
         <v>6</v>
@@ -2682,22 +2697,22 @@
     </row>
     <row r="10" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A10" s="59" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B10" s="62" t="s">
-        <v>83</v>
+        <v>86</v>
       </c>
       <c r="C10" s="62"/>
       <c r="D10" s="62"/>
       <c r="E10" s="62"/>
       <c r="F10" s="32" t="s">
-        <v>84</v>
+        <v>87</v>
       </c>
       <c r="G10" s="32"/>
       <c r="H10" s="32"/>
       <c r="I10" s="32"/>
       <c r="J10" s="56" t="s">
-        <v>85</v>
+        <v>88</v>
       </c>
       <c r="K10" s="56"/>
       <c r="L10" s="56"/>
@@ -2709,10 +2724,10 @@
     </row>
     <row r="11" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A11" s="59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B11" s="62" t="s">
-        <v>86</v>
+        <v>89</v>
       </c>
       <c r="C11" s="62"/>
       <c r="D11" s="62"/>
@@ -2730,7 +2745,7 @@
         <v>6</v>
       </c>
       <c r="J11" s="56" t="s">
-        <v>87</v>
+        <v>90</v>
       </c>
       <c r="K11" s="56"/>
       <c r="L11" s="56"/>
@@ -2742,7 +2757,7 @@
     </row>
     <row r="12" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A12" s="59" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>6</v>
@@ -2769,7 +2784,7 @@
         <v>6</v>
       </c>
       <c r="J12" s="56" t="s">
-        <v>88</v>
+        <v>91</v>
       </c>
       <c r="K12" s="56"/>
       <c r="L12" s="56"/>
@@ -2781,7 +2796,7 @@
     </row>
     <row r="13" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A13" s="59" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>6</v>
@@ -2808,7 +2823,7 @@
         <v>6</v>
       </c>
       <c r="J13" s="63" t="s">
-        <v>89</v>
+        <v>92</v>
       </c>
       <c r="K13" s="63"/>
       <c r="L13" s="63"/>
@@ -2820,7 +2835,7 @@
     </row>
     <row r="14" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A14" s="59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>6</v>
@@ -2847,7 +2862,7 @@
         <v>6</v>
       </c>
       <c r="J14" s="56" t="s">
-        <v>90</v>
+        <v>93</v>
       </c>
       <c r="K14" s="56"/>
       <c r="L14" s="56"/>
@@ -2859,7 +2874,7 @@
     </row>
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A15" s="59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B15" s="6" t="s">
         <v>6</v>
@@ -2886,7 +2901,7 @@
         <v>6</v>
       </c>
       <c r="J15" s="63" t="s">
-        <v>91</v>
+        <v>94</v>
       </c>
       <c r="K15" s="63"/>
       <c r="L15" s="63"/>
@@ -2898,7 +2913,7 @@
     </row>
     <row r="16" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B16" s="6" t="s">
         <v>6</v>
@@ -2925,7 +2940,7 @@
         <v>6</v>
       </c>
       <c r="J16" s="64" t="s">
-        <v>92</v>
+        <v>95</v>
       </c>
       <c r="K16" s="64"/>
       <c r="L16" s="64"/>
@@ -2937,10 +2952,10 @@
     </row>
     <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A17" s="65" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B17" s="66" t="s">
-        <v>93</v>
+        <v>96</v>
       </c>
       <c r="C17" s="66"/>
       <c r="D17" s="66"/>
@@ -2950,19 +2965,19 @@
       <c r="H17" s="66"/>
       <c r="I17" s="66"/>
       <c r="J17" s="64" t="s">
-        <v>94</v>
+        <v>97</v>
       </c>
       <c r="K17" s="64"/>
       <c r="L17" s="67" t="s">
-        <v>95</v>
+        <v>98</v>
       </c>
       <c r="M17" s="67"/>
       <c r="N17" s="67" t="s">
-        <v>96</v>
+        <v>99</v>
       </c>
       <c r="O17" s="67"/>
       <c r="P17" s="68" t="s">
-        <v>97</v>
+        <v>100</v>
       </c>
       <c r="Q17" s="68"/>
     </row>
@@ -3208,7 +3223,7 @@
     </row>
     <row r="27" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="B27" s="74"/>
       <c r="C27" s="28"/>
@@ -3229,7 +3244,7 @@
     </row>
     <row r="28" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="59" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="B28" s="62" t="n">
         <v>0.1234</v>
@@ -3256,7 +3271,7 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="B29" s="62" t="n">
         <v>128.788</v>
@@ -3283,7 +3298,7 @@
     </row>
     <row r="30" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="59" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="B30" s="74"/>
       <c r="C30" s="28"/>
@@ -3306,7 +3321,7 @@
     </row>
     <row r="31" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="59" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="B31" s="76"/>
       <c r="C31" s="23"/>
@@ -3329,7 +3344,7 @@
     </row>
     <row r="32" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="B32" s="77"/>
       <c r="C32" s="37"/>
@@ -3352,7 +3367,7 @@
     </row>
     <row r="33" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="B33" s="74"/>
       <c r="C33" s="28"/>
@@ -3375,7 +3390,7 @@
     </row>
     <row r="34" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A34" s="59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="B34" s="76"/>
       <c r="C34" s="23"/>
@@ -3386,7 +3401,7 @@
       <c r="H34" s="23"/>
       <c r="I34" s="23"/>
       <c r="J34" s="64" t="s">
-        <v>98</v>
+        <v>101</v>
       </c>
       <c r="K34" s="64"/>
       <c r="L34" s="64"/>
@@ -3398,10 +3413,10 @@
     </row>
     <row r="35" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A35" s="65" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="B35" s="66" t="s">
-        <v>99</v>
+        <v>102</v>
       </c>
       <c r="C35" s="66"/>
       <c r="D35" s="66"/>
@@ -3507,7 +3522,7 @@
   </sheetPr>
   <dimension ref="A6:W23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="B8" activeCellId="0" sqref="B8"/>
     </sheetView>
   </sheetViews>
@@ -3600,7 +3615,7 @@
       <c r="Q8" s="89"/>
       <c r="R8" s="90"/>
       <c r="S8" s="91" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="T8" s="91"/>
       <c r="U8" s="91"/>
@@ -3630,16 +3645,16 @@
       <c r="M9" s="94"/>
       <c r="N9" s="94"/>
       <c r="O9" s="95" t="s">
-        <v>101</v>
+        <v>104</v>
       </c>
       <c r="P9" s="96" t="s">
-        <v>102</v>
+        <v>105</v>
       </c>
       <c r="Q9" s="95" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="R9" s="97" t="s">
-        <v>103</v>
+        <v>106</v>
       </c>
       <c r="S9" s="91"/>
       <c r="T9" s="91"/>
@@ -3653,7 +3668,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="92" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="D10" s="92"/>
       <c r="E10" s="92"/>
@@ -3663,7 +3678,7 @@
       <c r="I10" s="92"/>
       <c r="J10" s="92"/>
       <c r="K10" s="99" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="L10" s="99"/>
       <c r="M10" s="99"/>
@@ -3673,7 +3688,7 @@
       <c r="Q10" s="99"/>
       <c r="R10" s="99"/>
       <c r="S10" s="100" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="T10" s="100"/>
       <c r="U10" s="100"/>
@@ -3686,7 +3701,7 @@
         <v>17</v>
       </c>
       <c r="C11" s="92" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D11" s="92"/>
       <c r="E11" s="92"/>
@@ -3696,7 +3711,7 @@
       <c r="I11" s="92"/>
       <c r="J11" s="92"/>
       <c r="K11" s="101" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L11" s="101"/>
       <c r="M11" s="101"/>
@@ -3717,7 +3732,7 @@
         <v>20</v>
       </c>
       <c r="C12" s="92" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D12" s="92"/>
       <c r="E12" s="92"/>
@@ -3727,7 +3742,7 @@
       <c r="I12" s="92"/>
       <c r="J12" s="92"/>
       <c r="K12" s="101" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L12" s="101"/>
       <c r="M12" s="101"/>
@@ -3764,7 +3779,7 @@
       <c r="Q13" s="71"/>
       <c r="R13" s="72"/>
       <c r="S13" s="100" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="T13" s="100"/>
       <c r="U13" s="100"/>
@@ -3801,7 +3816,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="83"/>
       <c r="B15" s="59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="74"/>
       <c r="D15" s="28"/>
@@ -3828,26 +3843,26 @@
     <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="83"/>
       <c r="B16" s="59" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C16" s="105" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="D16" s="105"/>
       <c r="E16" s="106" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="F16" s="106"/>
       <c r="G16" s="106" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="H16" s="106"/>
       <c r="I16" s="106" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="J16" s="106"/>
       <c r="K16" s="106" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="L16" s="106"/>
       <c r="M16" s="23"/>
@@ -3865,7 +3880,7 @@
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="83"/>
       <c r="B17" s="59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" s="77"/>
       <c r="D17" s="37"/>
@@ -3892,7 +3907,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="83"/>
       <c r="B18" s="59" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="28"/>
@@ -3919,7 +3934,7 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="83"/>
       <c r="B19" s="59" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="23"/>
@@ -3946,7 +3961,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="83"/>
       <c r="B20" s="59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" s="77"/>
       <c r="D20" s="37"/>
@@ -3973,7 +3988,7 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="83"/>
       <c r="B21" s="59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C21" s="74"/>
       <c r="D21" s="28"/>
@@ -4000,7 +4015,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="83"/>
       <c r="B22" s="59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="23"/>
@@ -4027,7 +4042,7 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="83"/>
       <c r="B23" s="65" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="109"/>
@@ -4090,7 +4105,7 @@
   </sheetPr>
   <dimension ref="A1:AL48"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="V20" activeCellId="0" sqref="V20"/>
     </sheetView>
   </sheetViews>
@@ -4847,7 +4862,7 @@
       <c r="AG21" s="8"/>
       <c r="AH21" s="8"/>
       <c r="AI21" s="51" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="AJ21" s="51"/>
       <c r="AK21" s="51"/>
@@ -5095,10 +5110,10 @@
       <c r="AC27" s="23"/>
       <c r="AD27" s="23"/>
       <c r="AE27" s="61" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="AF27" s="39" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="AG27" s="25"/>
       <c r="AH27" s="25"/>
@@ -5125,7 +5140,7 @@
       <c r="O28" s="23"/>
       <c r="P28" s="75"/>
       <c r="V28" s="59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="W28" s="74"/>
       <c r="X28" s="28"/>
@@ -5146,46 +5161,46 @@
     </row>
     <row r="29" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A29" s="130" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="B29" s="130"/>
       <c r="C29" s="130"/>
       <c r="D29" s="130"/>
       <c r="E29" s="131" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="F29" s="131"/>
       <c r="G29" s="131"/>
       <c r="H29" s="131"/>
       <c r="I29" s="131" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="J29" s="131"/>
       <c r="K29" s="131"/>
       <c r="L29" s="131"/>
       <c r="M29" s="132" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="N29" s="132"/>
       <c r="O29" s="132"/>
       <c r="P29" s="132"/>
       <c r="V29" s="59" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="W29" s="62" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="X29" s="62"/>
       <c r="Y29" s="62"/>
       <c r="Z29" s="62"/>
       <c r="AA29" s="32" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="AB29" s="32"/>
       <c r="AC29" s="32"/>
       <c r="AD29" s="32"/>
       <c r="AE29" s="56" t="s">
-        <v>43</v>
+        <v>46</v>
       </c>
       <c r="AF29" s="56"/>
       <c r="AG29" s="56"/>
@@ -5213,22 +5228,22 @@
       <c r="O30" s="23"/>
       <c r="P30" s="75"/>
       <c r="V30" s="59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="W30" s="62" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="X30" s="62"/>
       <c r="Y30" s="62"/>
       <c r="Z30" s="62"/>
       <c r="AA30" s="133" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="AB30" s="133"/>
       <c r="AC30" s="133"/>
       <c r="AD30" s="133"/>
       <c r="AE30" s="56" t="s">
-        <v>47</v>
+        <v>50</v>
       </c>
       <c r="AF30" s="56"/>
       <c r="AG30" s="56"/>
@@ -5256,7 +5271,7 @@
       <c r="O31" s="23"/>
       <c r="P31" s="75"/>
       <c r="V31" s="59" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="W31" s="74"/>
       <c r="X31" s="28"/>
@@ -5267,7 +5282,7 @@
       <c r="AC31" s="23"/>
       <c r="AD31" s="23"/>
       <c r="AE31" s="56" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="AF31" s="56"/>
       <c r="AG31" s="56"/>
@@ -5295,7 +5310,7 @@
       <c r="O32" s="23"/>
       <c r="P32" s="75"/>
       <c r="V32" s="59" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="W32" s="76"/>
       <c r="X32" s="23"/>
@@ -5306,7 +5321,7 @@
       <c r="AC32" s="23"/>
       <c r="AD32" s="23"/>
       <c r="AE32" s="63" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="AF32" s="63"/>
       <c r="AG32" s="63"/>
@@ -5334,7 +5349,7 @@
       <c r="O33" s="113"/>
       <c r="P33" s="114"/>
       <c r="V33" s="59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="W33" s="77"/>
       <c r="X33" s="37"/>
@@ -5345,7 +5360,7 @@
       <c r="AC33" s="37"/>
       <c r="AD33" s="37"/>
       <c r="AE33" s="56" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="AF33" s="56"/>
       <c r="AG33" s="56"/>
@@ -5373,7 +5388,7 @@
       <c r="O34" s="115"/>
       <c r="P34" s="116"/>
       <c r="V34" s="59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="W34" s="74"/>
       <c r="X34" s="28"/>
@@ -5384,7 +5399,7 @@
       <c r="AC34" s="23"/>
       <c r="AD34" s="23"/>
       <c r="AE34" s="63" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="AF34" s="63"/>
       <c r="AG34" s="63"/>
@@ -5412,7 +5427,7 @@
       <c r="O35" s="6"/>
       <c r="P35" s="117"/>
       <c r="V35" s="59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="W35" s="76"/>
       <c r="X35" s="23"/>
@@ -5429,7 +5444,7 @@
       <c r="AI35" s="23"/>
       <c r="AJ35" s="23"/>
       <c r="AK35" s="64" t="s">
-        <v>60</v>
+        <v>63</v>
       </c>
       <c r="AL35" s="64"/>
     </row>
@@ -5451,10 +5466,10 @@
       <c r="O36" s="118"/>
       <c r="P36" s="119"/>
       <c r="V36" s="65" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="W36" s="66" t="s">
-        <v>59</v>
+        <v>62</v>
       </c>
       <c r="X36" s="66"/>
       <c r="Y36" s="66"/>
@@ -5464,19 +5479,19 @@
       <c r="AC36" s="66"/>
       <c r="AD36" s="66"/>
       <c r="AE36" s="67" t="s">
-        <v>57</v>
+        <v>60</v>
       </c>
       <c r="AF36" s="67"/>
       <c r="AG36" s="67" t="s">
-        <v>61</v>
+        <v>64</v>
       </c>
       <c r="AH36" s="67"/>
       <c r="AI36" s="67" t="s">
-        <v>62</v>
+        <v>65</v>
       </c>
       <c r="AJ36" s="67"/>
       <c r="AK36" s="68" t="s">
-        <v>63</v>
+        <v>66</v>
       </c>
       <c r="AL36" s="68"/>
     </row>
@@ -5780,7 +5795,7 @@
   </sheetPr>
   <dimension ref="A6:W23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A2" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -5853,7 +5868,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="84" t="s">
-        <v>107</v>
+        <v>110</v>
       </c>
       <c r="D8" s="84"/>
       <c r="E8" s="84"/>
@@ -5877,7 +5892,7 @@
       <c r="Q8" s="122"/>
       <c r="R8" s="122"/>
       <c r="S8" s="91" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="T8" s="91"/>
       <c r="U8" s="91"/>
@@ -5889,7 +5904,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="92" t="s">
-        <v>106</v>
+        <v>109</v>
       </c>
       <c r="D9" s="92"/>
       <c r="E9" s="92"/>
@@ -5944,7 +5959,7 @@
       <c r="Q10" s="6"/>
       <c r="R10" s="128"/>
       <c r="S10" s="100" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="T10" s="100"/>
       <c r="U10" s="100"/>
@@ -6031,7 +6046,7 @@
       <c r="Q13" s="71"/>
       <c r="R13" s="72"/>
       <c r="S13" s="100" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="T13" s="100"/>
       <c r="U13" s="100"/>
@@ -6068,7 +6083,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="83"/>
       <c r="B15" s="59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="74"/>
       <c r="D15" s="28"/>
@@ -6095,7 +6110,7 @@
     <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="83"/>
       <c r="B16" s="59" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C16" s="105" t="s">
         <v>28</v>
@@ -6110,10 +6125,10 @@
         <v>32</v>
       </c>
       <c r="I16" s="95" t="s">
-        <v>35</v>
+        <v>37</v>
       </c>
       <c r="J16" s="95" t="s">
-        <v>38</v>
+        <v>40</v>
       </c>
       <c r="K16" s="23"/>
       <c r="L16" s="23"/>
@@ -6132,7 +6147,7 @@
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="83"/>
       <c r="B17" s="59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" s="77"/>
       <c r="D17" s="37"/>
@@ -6159,7 +6174,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="83"/>
       <c r="B18" s="59" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="28"/>
@@ -6186,7 +6201,7 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="83"/>
       <c r="B19" s="59" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="23"/>
@@ -6213,28 +6228,28 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A20" s="83"/>
       <c r="B20" s="59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" s="130" t="s">
-        <v>41</v>
+        <v>44</v>
       </c>
       <c r="D20" s="130"/>
       <c r="E20" s="130"/>
       <c r="F20" s="130"/>
       <c r="G20" s="131" t="s">
-        <v>42</v>
+        <v>45</v>
       </c>
       <c r="H20" s="131"/>
       <c r="I20" s="131"/>
       <c r="J20" s="131"/>
       <c r="K20" s="131" t="s">
-        <v>45</v>
+        <v>48</v>
       </c>
       <c r="L20" s="131"/>
       <c r="M20" s="131"/>
       <c r="N20" s="131"/>
       <c r="O20" s="132" t="s">
-        <v>46</v>
+        <v>49</v>
       </c>
       <c r="P20" s="132"/>
       <c r="Q20" s="132"/>
@@ -6248,7 +6263,7 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="83"/>
       <c r="B21" s="59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C21" s="74"/>
       <c r="D21" s="28"/>
@@ -6275,7 +6290,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="83"/>
       <c r="B22" s="59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="23"/>
@@ -6302,7 +6317,7 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="83"/>
       <c r="B23" s="65" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="109"/>
@@ -6366,7 +6381,7 @@
   </sheetPr>
   <dimension ref="A6:W23"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A4" colorId="64" zoomScale="120" zoomScaleNormal="120" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C8" activeCellId="0" sqref="C8"/>
     </sheetView>
   </sheetViews>
@@ -6438,7 +6453,7 @@
         <v>6</v>
       </c>
       <c r="C8" s="84" t="s">
-        <v>108</v>
+        <v>111</v>
       </c>
       <c r="D8" s="84"/>
       <c r="E8" s="84"/>
@@ -6448,7 +6463,7 @@
       <c r="I8" s="84"/>
       <c r="J8" s="84"/>
       <c r="K8" s="134" t="s">
-        <v>109</v>
+        <v>112</v>
       </c>
       <c r="L8" s="134"/>
       <c r="M8" s="134"/>
@@ -6458,7 +6473,7 @@
       <c r="Q8" s="134"/>
       <c r="R8" s="134"/>
       <c r="S8" s="91" t="s">
-        <v>100</v>
+        <v>103</v>
       </c>
       <c r="T8" s="91"/>
       <c r="U8" s="91"/>
@@ -6470,7 +6485,7 @@
         <v>11</v>
       </c>
       <c r="C9" s="92" t="s">
-        <v>49</v>
+        <v>52</v>
       </c>
       <c r="D9" s="92"/>
       <c r="E9" s="92"/>
@@ -6480,7 +6495,7 @@
       <c r="I9" s="92"/>
       <c r="J9" s="92"/>
       <c r="K9" s="135" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="L9" s="135"/>
       <c r="M9" s="135"/>
@@ -6501,7 +6516,7 @@
         <v>14</v>
       </c>
       <c r="C10" s="92" t="s">
-        <v>53</v>
+        <v>56</v>
       </c>
       <c r="D10" s="92"/>
       <c r="E10" s="92"/>
@@ -6511,7 +6526,7 @@
       <c r="I10" s="92"/>
       <c r="J10" s="92"/>
       <c r="K10" s="99" t="s">
-        <v>55</v>
+        <v>58</v>
       </c>
       <c r="L10" s="99"/>
       <c r="M10" s="99"/>
@@ -6521,7 +6536,7 @@
       <c r="Q10" s="99"/>
       <c r="R10" s="99"/>
       <c r="S10" s="100" t="s">
-        <v>104</v>
+        <v>107</v>
       </c>
       <c r="T10" s="100"/>
       <c r="U10" s="100"/>
@@ -6604,7 +6619,7 @@
       <c r="Q13" s="71"/>
       <c r="R13" s="72"/>
       <c r="S13" s="100" t="s">
-        <v>105</v>
+        <v>108</v>
       </c>
       <c r="T13" s="100"/>
       <c r="U13" s="100"/>
@@ -6641,7 +6656,7 @@
     <row r="15" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="83"/>
       <c r="B15" s="59" t="s">
-        <v>39</v>
+        <v>41</v>
       </c>
       <c r="C15" s="74"/>
       <c r="D15" s="28"/>
@@ -6668,7 +6683,7 @@
     <row r="16" customFormat="false" ht="22.5" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A16" s="83"/>
       <c r="B16" s="59" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
       <c r="C16" s="76"/>
       <c r="D16" s="23"/>
@@ -6695,7 +6710,7 @@
     <row r="17" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="83"/>
       <c r="B17" s="59" t="s">
-        <v>44</v>
+        <v>47</v>
       </c>
       <c r="C17" s="77"/>
       <c r="D17" s="37"/>
@@ -6722,7 +6737,7 @@
     <row r="18" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="83"/>
       <c r="B18" s="59" t="s">
-        <v>48</v>
+        <v>51</v>
       </c>
       <c r="C18" s="74"/>
       <c r="D18" s="28"/>
@@ -6749,7 +6764,7 @@
     <row r="19" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="83"/>
       <c r="B19" s="59" t="s">
-        <v>50</v>
+        <v>53</v>
       </c>
       <c r="C19" s="76"/>
       <c r="D19" s="23"/>
@@ -6776,7 +6791,7 @@
     <row r="20" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="83"/>
       <c r="B20" s="59" t="s">
-        <v>52</v>
+        <v>55</v>
       </c>
       <c r="C20" s="77"/>
       <c r="D20" s="37"/>
@@ -6803,7 +6818,7 @@
     <row r="21" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="83"/>
       <c r="B21" s="59" t="s">
-        <v>54</v>
+        <v>57</v>
       </c>
       <c r="C21" s="74"/>
       <c r="D21" s="28"/>
@@ -6830,7 +6845,7 @@
     <row r="22" customFormat="false" ht="15" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="83"/>
       <c r="B22" s="59" t="s">
-        <v>56</v>
+        <v>59</v>
       </c>
       <c r="C22" s="76"/>
       <c r="D22" s="23"/>
@@ -6857,7 +6872,7 @@
     <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="83"/>
       <c r="B23" s="65" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C23" s="108"/>
       <c r="D23" s="109"/>

</xml_diff>